<commit_message>
Add LeaderID in LeaderCardPoolDatabase.xlsx
</commit_message>
<xml_diff>
--- a/Resources/LeaderCardPoolDatabase.xlsx
+++ b/Resources/LeaderCardPoolDatabase.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$130</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$F$130</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="90">
   <si>
     <t>Emhyr var Emreis: His Imperial Majesty</t>
   </si>
@@ -317,6 +317,10 @@
   </si>
   <si>
     <t>Eredin Bréacc Glas: The Treacherous</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>leaderID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -642,391 +646,454 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1"/>
-    <col min="2" max="2" width="51.25" customWidth="1"/>
-    <col min="3" max="3" width="99.125" customWidth="1"/>
-    <col min="4" max="4" width="9.875" customWidth="1"/>
-    <col min="5" max="5" width="55.25" customWidth="1"/>
-    <col min="6" max="6" width="9.375" customWidth="1"/>
-    <col min="7" max="7" width="35.25" customWidth="1"/>
+    <col min="2" max="2" width="31" customWidth="1"/>
+    <col min="3" max="3" width="51.25" customWidth="1"/>
+    <col min="4" max="4" width="99.125" customWidth="1"/>
+    <col min="5" max="5" width="9.875" customWidth="1"/>
+    <col min="6" max="6" width="55.25" customWidth="1"/>
+    <col min="7" max="7" width="9.375" customWidth="1"/>
+    <col min="8" max="8" width="35.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>68</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>42</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>69</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>43</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>70</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>44</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>71</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>45</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>72</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>50</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>17</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>73</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>38</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>19</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>74</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>39</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>19</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>75</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>40</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>19</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>76</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>41</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>19</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>77</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>32</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>19</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
         <v>9</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>78</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>33</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>20</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
         <v>10</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>79</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>34</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>20</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
         <v>11</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>80</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>35</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>20</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
         <v>12</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>81</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>36</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>20</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
         <v>13</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>82</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>37</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>20</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
         <v>22</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>83</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>31</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>29</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="18" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
         <v>23</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>84</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>24</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>29</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="19" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
         <v>25</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>85</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>26</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>29</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="20" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
         <v>27</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>86</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>28</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>29</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="21" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
         <v>88</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>87</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>30</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>29</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fix a serious typing error;
</commit_message>
<xml_diff>
--- a/Resources/LeaderCardPoolDatabase.xlsx
+++ b/Resources/LeaderCardPoolDatabase.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -78,12 +78,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Nilfgaarian</t>
-  </si>
-  <si>
-    <t>Emhyr var Emreis: Emperor of Nilfgaarian</t>
-  </si>
-  <si>
     <t>Northern</t>
   </si>
   <si>
@@ -259,9 +253,6 @@
     <t>Leader\Emhyr var Emreis: His Imperial Majesty.png</t>
   </si>
   <si>
-    <t>Leader\Emhyr var Emreis: Emperor of Nilfgaarian.png</t>
-  </si>
-  <si>
     <t>Leader\Emhyr var Emreis: the White Flame.png</t>
   </si>
   <si>
@@ -322,6 +313,15 @@
   <si>
     <t>leaderID</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nilfgaardian</t>
+  </si>
+  <si>
+    <t>Emhyr var Emreis: Emperor of Nilfgaardian</t>
+  </si>
+  <si>
+    <t>Leader\Emhyr var Emreis: Emperor of Nilfgaardian.png</t>
   </si>
 </sst>
 </file>
@@ -649,7 +649,7 @@
   <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -665,7 +665,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B1" t="s">
         <v>15</v>
@@ -674,13 +674,13 @@
         <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
         <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -691,16 +691,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="F2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -708,19 +708,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>88</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="F3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -731,16 +731,16 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -751,16 +751,16 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="F5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -771,16 +771,16 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="F6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -791,16 +791,16 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -811,16 +811,16 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -831,16 +831,16 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -851,16 +851,16 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -871,16 +871,16 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -891,16 +891,16 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -911,16 +911,16 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -931,16 +931,16 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -951,16 +951,16 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -971,16 +971,16 @@
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -988,19 +988,19 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1008,19 +1008,19 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1028,19 +1028,19 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1048,19 +1048,19 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" t="s">
         <v>27</v>
       </c>
-      <c r="C20" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" t="s">
-        <v>29</v>
-      </c>
       <c r="F20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1068,19 +1068,19 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C21" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
finishing 2nd scenes of collection connected interfaces
</commit_message>
<xml_diff>
--- a/Resources/LeaderCardPoolDatabase.xlsx
+++ b/Resources/LeaderCardPoolDatabase.xlsx
@@ -156,9 +156,6 @@
     <t>Look at 3 random cards from your opponent's hand.</t>
   </si>
   <si>
-    <t>Cancel your opponent's Leader Ability.</t>
-  </si>
-  <si>
     <t>Draw a card from your opponent's discard pile.</t>
   </si>
   <si>
@@ -250,78 +247,81 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Leader\Emhyr var Emreis: His Imperial Majesty.png</t>
-  </si>
-  <si>
-    <t>Leader\Emhyr var Emreis: the White Flame.png</t>
-  </si>
-  <si>
-    <t>Leader\Emhyr var Emreis: The Relentless.png</t>
-  </si>
-  <si>
-    <t>Leader\Emhyr var Emreis: Invader of the North.png</t>
-  </si>
-  <si>
-    <t>Leader\Foltest: King of Temeria.png</t>
-  </si>
-  <si>
-    <t>Leader\Foltest: Lord Commander of the North.png</t>
-  </si>
-  <si>
-    <t>Leader\Foltest: The Siegemaster.png</t>
-  </si>
-  <si>
-    <t>Leader\Foltest: The Steel-Forged.png</t>
-  </si>
-  <si>
-    <t>Leader\Foltest: Son of Medell.png</t>
-  </si>
-  <si>
-    <t>Leader\Francesca Findabair: Pureblood Elf.png</t>
-  </si>
-  <si>
-    <t>Leader\Francesca Findabair: Daisy of the Valley.png</t>
-  </si>
-  <si>
-    <t>Leader\Francesca Findabair: the Beautiful.png</t>
-  </si>
-  <si>
-    <t>Leader\Francesca Findabair: Queen of Dol Blathanna.png</t>
-  </si>
-  <si>
-    <t>Leader\Francesca Findabair: Hope of the Aen Seidhe.png</t>
-  </si>
-  <si>
-    <t>Leader\Eredin: King of the Wild Hunt.png</t>
-  </si>
-  <si>
-    <t>Leader\Eredin: Commander of the Red Riders.png</t>
-  </si>
-  <si>
-    <t>Leader\Eredin: Destroyer of Worlds.png</t>
-  </si>
-  <si>
-    <t>Leader\Eredin: Bringer of Death.png</t>
-  </si>
-  <si>
-    <t>Leader\Eredin Bréacc Glas: The Treacherous.png</t>
-  </si>
-  <si>
     <t>Eredin Bréacc Glas: The Treacherous</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>leaderID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Nilfgaardian</t>
   </si>
   <si>
-    <t>Emhyr var Emreis: Emperor of Nilfgaardian</t>
-  </si>
-  <si>
-    <t>Leader\Emhyr var Emreis: Emperor of Nilfgaardian.png</t>
+    <t>Emhyr var Emreis: Emperor of Nilfgaard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LeadersID</t>
+  </si>
+  <si>
+    <t>Leaders/Emhyr var Emreis His Imperial Majesty.png</t>
+  </si>
+  <si>
+    <t>Leaders/Emhyr var Emreis Emperor of Nilfgaard.png</t>
+  </si>
+  <si>
+    <t>Leaders/Emhyr var Emreis the White Flame.png</t>
+  </si>
+  <si>
+    <t>Cancel your opponent's Leaders Ability.</t>
+  </si>
+  <si>
+    <t>Leaders/Emhyr var Emreis The Relentless.png</t>
+  </si>
+  <si>
+    <t>Leaders/Emhyr var Emreis Invader of the North.png</t>
+  </si>
+  <si>
+    <t>Leaders/Foltest King of Temeria.png</t>
+  </si>
+  <si>
+    <t>Leaders/Foltest Lord Commander of the North.png</t>
+  </si>
+  <si>
+    <t>Leaders/Foltest The Siegemaster.png</t>
+  </si>
+  <si>
+    <t>Leaders/Foltest The Steel-Forged.png</t>
+  </si>
+  <si>
+    <t>Leaders/Foltest Son of Medell.png</t>
+  </si>
+  <si>
+    <t>Leaders/Francesca Findabair Pureblood Elf.png</t>
+  </si>
+  <si>
+    <t>Leaders/Francesca Findabair Daisy of the Valley.png</t>
+  </si>
+  <si>
+    <t>Leaders/Francesca Findabair the Beautiful.png</t>
+  </si>
+  <si>
+    <t>Leaders/Francesca Findabair Queen of Dol Blathanna.png</t>
+  </si>
+  <si>
+    <t>Leaders/Francesca Findabair Hope of the Aen Seidhe.png</t>
+  </si>
+  <si>
+    <t>Leaders/Eredin King of the Wild Hunt.png</t>
+  </si>
+  <si>
+    <t>Leaders/Eredin Commander of the Red Riders.png</t>
+  </si>
+  <si>
+    <t>Leaders/Eredin Destroyer of Worlds.png</t>
+  </si>
+  <si>
+    <t>Leaders/Eredin Bringer of Death.png</t>
+  </si>
+  <si>
+    <t>Leaders/Eredin Bréacc Glas The Treacherous.png</t>
   </si>
 </sst>
 </file>
@@ -649,14 +649,15 @@
   <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="51.25" customWidth="1"/>
-    <col min="4" max="4" width="99.125" customWidth="1"/>
+    <col min="1" max="1" width="4.25" customWidth="1"/>
+    <col min="2" max="2" width="40.625" customWidth="1"/>
+    <col min="3" max="3" width="48.875" customWidth="1"/>
+    <col min="4" max="4" width="17.25" customWidth="1"/>
     <col min="5" max="5" width="9.875" customWidth="1"/>
     <col min="6" max="6" width="55.25" customWidth="1"/>
     <col min="7" max="7" width="9.375" customWidth="1"/>
@@ -665,7 +666,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="B1" t="s">
         <v>15</v>
@@ -680,7 +681,7 @@
         <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -691,16 +692,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D2" t="s">
         <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -708,19 +709,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="D3" t="s">
         <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="F3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -731,16 +732,16 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="E4" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="F4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -751,16 +752,16 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="F5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -771,16 +772,16 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" t="s">
         <v>48</v>
-      </c>
-      <c r="E6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F6" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -791,7 +792,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D7" t="s">
         <v>36</v>
@@ -800,7 +801,7 @@
         <v>17</v>
       </c>
       <c r="F7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -811,7 +812,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D8" t="s">
         <v>37</v>
@@ -820,7 +821,7 @@
         <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -831,7 +832,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="D9" t="s">
         <v>38</v>
@@ -840,7 +841,7 @@
         <v>17</v>
       </c>
       <c r="F9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -851,7 +852,7 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D10" t="s">
         <v>39</v>
@@ -860,7 +861,7 @@
         <v>17</v>
       </c>
       <c r="F10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -871,7 +872,7 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D11" t="s">
         <v>30</v>
@@ -880,7 +881,7 @@
         <v>17</v>
       </c>
       <c r="F11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -891,7 +892,7 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D12" t="s">
         <v>31</v>
@@ -900,7 +901,7 @@
         <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -911,7 +912,7 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D13" t="s">
         <v>32</v>
@@ -920,7 +921,7 @@
         <v>18</v>
       </c>
       <c r="F13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -931,7 +932,7 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D14" t="s">
         <v>33</v>
@@ -940,7 +941,7 @@
         <v>18</v>
       </c>
       <c r="F14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -951,7 +952,7 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D15" t="s">
         <v>34</v>
@@ -960,7 +961,7 @@
         <v>18</v>
       </c>
       <c r="F15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -971,7 +972,7 @@
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D16" t="s">
         <v>35</v>
@@ -980,7 +981,7 @@
         <v>18</v>
       </c>
       <c r="F16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -991,7 +992,7 @@
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D17" t="s">
         <v>29</v>
@@ -1000,7 +1001,7 @@
         <v>27</v>
       </c>
       <c r="F17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1011,7 +1012,7 @@
         <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D18" t="s">
         <v>22</v>
@@ -1020,7 +1021,7 @@
         <v>27</v>
       </c>
       <c r="F18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1031,7 +1032,7 @@
         <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D19" t="s">
         <v>24</v>
@@ -1040,7 +1041,7 @@
         <v>27</v>
       </c>
       <c r="F19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1051,7 +1052,7 @@
         <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="D20" t="s">
         <v>26</v>
@@ -1060,7 +1061,7 @@
         <v>27</v>
       </c>
       <c r="F20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1068,10 +1069,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="C21" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D21" t="s">
         <v>28</v>
@@ -1080,7 +1081,7 @@
         <v>27</v>
       </c>
       <c r="F21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fix annother typing error in the interface of leaderCard
</commit_message>
<xml_diff>
--- a/Resources/LeaderCardPoolDatabase.xlsx
+++ b/Resources/LeaderCardPoolDatabase.xlsx
@@ -294,43 +294,43 @@
     <t>Leaders/Foltest Son of Medell.png</t>
   </si>
   <si>
+    <t>Leaders/Eredin Destroyer of Worlds.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Leaders/Eredin Commander of the Red Riders.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Leaders/Eredin Breacc Glas The Treacherous.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Leaders/Francesca Findabair Daisy of The Valle.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Leaders/Francesca Findabair Hope of the Aen Seidhe.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Leaders/Francesca Findabair Pureblood Elf.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Leaders/Francesca Findabair Queen of Dol Blathanna.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Leaders/Francesca Findabair the Beautiful.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Leaders/Eredin Bringer of Death.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Leaders/Eredin King of the Wild Hunt.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Leaders/Eredin Destroyer of Worlds.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Leaders/Eredin Commander of the Red Riders.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Leaders/Eredin Bringer of Death.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Leaders/Eredin Breacc Glas The Treacherous.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Leaders/Francesca Findabair Daisy of The Valle.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Leaders/Francesca Findabair Hope of the Aen Seidhe.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Leaders/Francesca Findabair Pureblood Elf.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Leaders/Francesca Findabair Queen of Dol Blathanna.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Leaders/Francesca Findabair the Beautiful.png</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -659,7 +659,7 @@
   <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -902,7 +902,7 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D12" t="s">
         <v>31</v>
@@ -922,7 +922,7 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D13" t="s">
         <v>32</v>
@@ -942,7 +942,7 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D14" t="s">
         <v>33</v>
@@ -962,7 +962,7 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D15" t="s">
         <v>34</v>
@@ -982,7 +982,7 @@
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D16" t="s">
         <v>35</v>
@@ -1002,7 +1002,7 @@
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="D17" t="s">
         <v>29</v>
@@ -1022,7 +1022,7 @@
         <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D18" t="s">
         <v>22</v>
@@ -1042,7 +1042,7 @@
         <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D19" t="s">
         <v>24</v>
@@ -1062,7 +1062,7 @@
         <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="D20" t="s">
         <v>26</v>
@@ -1082,7 +1082,7 @@
         <v>65</v>
       </c>
       <c r="C21" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D21" t="s">
         <v>28</v>

</xml_diff>